<commit_message>
added data visualization html
</commit_message>
<xml_diff>
--- a/data/gas_prices.xlsx
+++ b/data/gas_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I929"/>
+  <dimension ref="A1:I1009"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36849,10 +36849,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" t="inlineStr">
-        <is>
-          <t>65515</t>
-        </is>
+      <c r="A910" t="n">
+        <v>65515</v>
       </c>
       <c r="B910" t="inlineStr">
         <is>
@@ -36892,10 +36890,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" t="inlineStr">
-        <is>
-          <t>77205</t>
-        </is>
+      <c r="A911" t="n">
+        <v>77205</v>
       </c>
       <c r="B911" t="inlineStr">
         <is>
@@ -36935,10 +36931,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" t="inlineStr">
-        <is>
-          <t>77223</t>
-        </is>
+      <c r="A912" t="n">
+        <v>77223</v>
       </c>
       <c r="B912" t="inlineStr">
         <is>
@@ -36978,10 +36972,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" t="inlineStr">
-        <is>
-          <t>65514</t>
-        </is>
+      <c r="A913" t="n">
+        <v>65514</v>
       </c>
       <c r="B913" t="inlineStr">
         <is>
@@ -37021,10 +37013,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" t="inlineStr">
-        <is>
-          <t>77232</t>
-        </is>
+      <c r="A914" t="n">
+        <v>77232</v>
       </c>
       <c r="B914" t="inlineStr">
         <is>
@@ -37064,10 +37054,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" t="inlineStr">
-        <is>
-          <t>77202</t>
-        </is>
+      <c r="A915" t="n">
+        <v>77202</v>
       </c>
       <c r="B915" t="inlineStr">
         <is>
@@ -37107,10 +37095,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" t="inlineStr">
-        <is>
-          <t>86650</t>
-        </is>
+      <c r="A916" t="n">
+        <v>86650</v>
       </c>
       <c r="B916" t="inlineStr">
         <is>
@@ -37150,10 +37136,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" t="inlineStr">
-        <is>
-          <t>77218</t>
-        </is>
+      <c r="A917" t="n">
+        <v>77218</v>
       </c>
       <c r="B917" t="inlineStr">
         <is>
@@ -37193,10 +37177,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" t="inlineStr">
-        <is>
-          <t>77243</t>
-        </is>
+      <c r="A918" t="n">
+        <v>77243</v>
       </c>
       <c r="B918" t="inlineStr">
         <is>
@@ -37236,10 +37218,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" t="inlineStr">
-        <is>
-          <t>77235</t>
-        </is>
+      <c r="A919" t="n">
+        <v>77235</v>
       </c>
       <c r="B919" t="inlineStr">
         <is>
@@ -37279,10 +37259,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" t="inlineStr">
-        <is>
-          <t>77228</t>
-        </is>
+      <c r="A920" t="n">
+        <v>77228</v>
       </c>
       <c r="B920" t="inlineStr">
         <is>
@@ -37322,10 +37300,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" t="inlineStr">
-        <is>
-          <t>69163</t>
-        </is>
+      <c r="A921" t="n">
+        <v>69163</v>
       </c>
       <c r="B921" t="inlineStr">
         <is>
@@ -37365,10 +37341,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" t="inlineStr">
-        <is>
-          <t>109205</t>
-        </is>
+      <c r="A922" t="n">
+        <v>109205</v>
       </c>
       <c r="B922" t="inlineStr">
         <is>
@@ -37408,10 +37382,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" t="inlineStr">
-        <is>
-          <t>65512</t>
-        </is>
+      <c r="A923" t="n">
+        <v>65512</v>
       </c>
       <c r="B923" t="inlineStr">
         <is>
@@ -37451,10 +37423,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" t="inlineStr">
-        <is>
-          <t>83384</t>
-        </is>
+      <c r="A924" t="n">
+        <v>83384</v>
       </c>
       <c r="B924" t="inlineStr">
         <is>
@@ -37494,10 +37464,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" t="inlineStr">
-        <is>
-          <t>77015</t>
-        </is>
+      <c r="A925" t="n">
+        <v>77015</v>
       </c>
       <c r="B925" t="inlineStr">
         <is>
@@ -37537,10 +37505,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" t="inlineStr">
-        <is>
-          <t>107728</t>
-        </is>
+      <c r="A926" t="n">
+        <v>107728</v>
       </c>
       <c r="B926" t="inlineStr">
         <is>
@@ -37580,10 +37546,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" t="inlineStr">
-        <is>
-          <t>65572</t>
-        </is>
+      <c r="A927" t="n">
+        <v>65572</v>
       </c>
       <c r="B927" t="inlineStr">
         <is>
@@ -37623,10 +37587,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" t="inlineStr">
-        <is>
-          <t>65511</t>
-        </is>
+      <c r="A928" t="n">
+        <v>65511</v>
       </c>
       <c r="B928" t="inlineStr">
         <is>
@@ -37666,10 +37628,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" t="inlineStr">
-        <is>
-          <t>65556</t>
-        </is>
+      <c r="A929" t="n">
+        <v>65556</v>
       </c>
       <c r="B929" t="inlineStr">
         <is>
@@ -37705,6 +37665,3308 @@
         </is>
       </c>
       <c r="I929" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="n">
+        <v>65542</v>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>3250 MacDonald St</t>
+        </is>
+      </c>
+      <c r="D930" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2573819, 'Longitude': -123.1680407}</t>
+        </is>
+      </c>
+      <c r="E930" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F930" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:36:26.079Z</t>
+        </is>
+      </c>
+      <c r="G930" t="n">
+        <v>157.9</v>
+      </c>
+      <c r="H930" t="inlineStr">
+        <is>
+          <t>2025-06-01T23:23:24.418Z</t>
+        </is>
+      </c>
+      <c r="I930" t="n">
+        <v>186.9</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="n">
+        <v>65533</v>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>4615 Arbutus St</t>
+        </is>
+      </c>
+      <c r="D931" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2449719, 'Longitude': -123.1540385}</t>
+        </is>
+      </c>
+      <c r="E931" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F931" t="inlineStr">
+        <is>
+          <t>2025-06-02T21:15:28.347Z</t>
+        </is>
+      </c>
+      <c r="G931" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H931" t="inlineStr">
+        <is>
+          <t>2025-06-02T15:54:11.437Z</t>
+        </is>
+      </c>
+      <c r="I931" t="n">
+        <v>185.9</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="n">
+        <v>83068</v>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>3205 Arbutus St</t>
+        </is>
+      </c>
+      <c r="D932" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.256927568207, 'Longitude': -123.153288960457}</t>
+        </is>
+      </c>
+      <c r="E932" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F932" t="inlineStr"/>
+      <c r="G932" t="inlineStr"/>
+      <c r="H932" t="inlineStr"/>
+      <c r="I932" t="inlineStr"/>
+    </row>
+    <row r="933">
+      <c r="A933" t="n">
+        <v>65562</v>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>2808 W Broadway</t>
+        </is>
+      </c>
+      <c r="D933" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.263883932125, 'Longitude': -123.168604373932}</t>
+        </is>
+      </c>
+      <c r="E933" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F933" t="inlineStr">
+        <is>
+          <t>2025-06-02T23:25:05.995Z</t>
+        </is>
+      </c>
+      <c r="G933" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H933" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:12:18.248Z</t>
+        </is>
+      </c>
+      <c r="I933" t="n">
+        <v>184.9</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="n">
+        <v>113305</v>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>3596 W 41st Ave</t>
+        </is>
+      </c>
+      <c r="D934" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234385296079, 'Longitude': -123.184762001038}</t>
+        </is>
+      </c>
+      <c r="E934" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F934" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:50:11.380Z</t>
+        </is>
+      </c>
+      <c r="G934" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H934" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:48:59.863Z</t>
+        </is>
+      </c>
+      <c r="I934" t="n">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="n">
+        <v>65570</v>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>2103 W Broadway</t>
+        </is>
+      </c>
+      <c r="D935" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.264135981257, 'Longitude': -123.153326511383}</t>
+        </is>
+      </c>
+      <c r="E935" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F935" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:07:49.260Z</t>
+        </is>
+      </c>
+      <c r="G935" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="H935" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:07:49.291Z</t>
+        </is>
+      </c>
+      <c r="I935" t="n">
+        <v>180.9</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="n">
+        <v>65554</v>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>1795 W Broadway</t>
+        </is>
+      </c>
+      <c r="D936" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.264037962303, 'Longitude': -123.145408630371}</t>
+        </is>
+      </c>
+      <c r="E936" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F936" t="inlineStr">
+        <is>
+          <t>2025-06-02T21:11:10.996Z</t>
+        </is>
+      </c>
+      <c r="G936" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H936" t="inlineStr">
+        <is>
+          <t>2025-06-02T19:02:10.652Z</t>
+        </is>
+      </c>
+      <c r="I936" t="n">
+        <v>186.9</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="n">
+        <v>65571</v>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>4314 W 10th Ave</t>
+        </is>
+      </c>
+      <c r="D937" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.263533861752, 'Longitude': -123.203430175781}</t>
+        </is>
+      </c>
+      <c r="E937" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F937" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:45:39.313Z</t>
+        </is>
+      </c>
+      <c r="G937" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H937" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:47:15.048Z</t>
+        </is>
+      </c>
+      <c r="I937" t="n">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="n">
+        <v>65565</v>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>1896 W 4th Ave</t>
+        </is>
+      </c>
+      <c r="D938" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.267881559667, 'Longitude': -123.14772605896}</t>
+        </is>
+      </c>
+      <c r="E938" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F938" t="inlineStr">
+        <is>
+          <t>2025-06-02T23:42:40.825Z</t>
+        </is>
+      </c>
+      <c r="G938" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H938" t="inlineStr">
+        <is>
+          <t>2025-06-02T01:28:36.672Z</t>
+        </is>
+      </c>
+      <c r="I938" t="n">
+        <v>182.9</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="n">
+        <v>32376</v>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>1503 W 41st Ave</t>
+        </is>
+      </c>
+      <c r="D939" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234634576953, 'Longitude': -123.139971792698}</t>
+        </is>
+      </c>
+      <c r="E939" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F939" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:59:05.460Z</t>
+        </is>
+      </c>
+      <c r="G939" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H939" t="inlineStr">
+        <is>
+          <t>2025-06-02T18:05:42.342Z</t>
+        </is>
+      </c>
+      <c r="I939" t="n">
+        <v>184.9</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="n">
+        <v>65549</v>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>5702 Granville St</t>
+        </is>
+      </c>
+      <c r="D940" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234036184118, 'Longitude': -123.139244914055}</t>
+        </is>
+      </c>
+      <c r="E940" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F940" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:59:01.507Z</t>
+        </is>
+      </c>
+      <c r="G940" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H940" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:05:28.254Z</t>
+        </is>
+      </c>
+      <c r="I940" t="n">
+        <v>186.9</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="n">
+        <v>65543</v>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>1900 Burrard St</t>
+        </is>
+      </c>
+      <c r="D941" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2685375, 'Longitude': -123.1453067}</t>
+        </is>
+      </c>
+      <c r="E941" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F941" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:12:13.980Z</t>
+        </is>
+      </c>
+      <c r="G941" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H941" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:12:14.011Z</t>
+        </is>
+      </c>
+      <c r="I941" t="n">
+        <v>184.9</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="n">
+        <v>65563</v>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>1743 Burrard St</t>
+        </is>
+      </c>
+      <c r="D942" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.270429790667, 'Longitude': -123.145886063576}</t>
+        </is>
+      </c>
+      <c r="E942" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F942" t="inlineStr">
+        <is>
+          <t>2025-06-02T21:08:39.939Z</t>
+        </is>
+      </c>
+      <c r="G942" t="n">
+        <v>158.9</v>
+      </c>
+      <c r="H942" t="inlineStr">
+        <is>
+          <t>2025-06-02T01:28:48.940Z</t>
+        </is>
+      </c>
+      <c r="I942" t="n">
+        <v>181.9</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="n">
+        <v>72747</v>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>1010 W King Edward Ave</t>
+        </is>
+      </c>
+      <c r="D943" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.249188, 'Longitude': -123.127767}</t>
+        </is>
+      </c>
+      <c r="E943" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F943" t="inlineStr">
+        <is>
+          <t>2025-06-02T21:57:58.148Z</t>
+        </is>
+      </c>
+      <c r="G943" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H943" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:31:24.442Z</t>
+        </is>
+      </c>
+      <c r="I943" t="n">
+        <v>204.9</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="n">
+        <v>32375</v>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>4110 Oak St</t>
+        </is>
+      </c>
+      <c r="D944" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.24894071957, 'Longitude': -123.127040863037}</t>
+        </is>
+      </c>
+      <c r="E944" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F944" t="inlineStr">
+        <is>
+          <t>2025-06-02T21:57:35.837Z</t>
+        </is>
+      </c>
+      <c r="G944" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H944" t="inlineStr">
+        <is>
+          <t>2025-06-02T15:53:51.165Z</t>
+        </is>
+      </c>
+      <c r="I944" t="n">
+        <v>208.9</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="n">
+        <v>65564</v>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>5680 Oak St</t>
+        </is>
+      </c>
+      <c r="D945" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234217162181, 'Longitude': -123.127684593201}</t>
+        </is>
+      </c>
+      <c r="E945" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F945" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:12:23.723Z</t>
+        </is>
+      </c>
+      <c r="G945" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H945" t="inlineStr">
+        <is>
+          <t>2025-06-02T18:57:18.658Z</t>
+        </is>
+      </c>
+      <c r="I945" t="n">
+        <v>184.9</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="n">
+        <v>32372</v>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>6525 Oak St</t>
+        </is>
+      </c>
+      <c r="D946" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.226226639452, 'Longitude': -123.128687739372}</t>
+        </is>
+      </c>
+      <c r="E946" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F946" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:26:03.757Z</t>
+        </is>
+      </c>
+      <c r="G946" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H946" t="inlineStr"/>
+      <c r="I946" t="inlineStr"/>
+    </row>
+    <row r="947">
+      <c r="A947" t="n">
+        <v>9707</v>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>1205 Burrard St</t>
+        </is>
+      </c>
+      <c r="D947" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.279145231489, 'Longitude': -123.12982365489}</t>
+        </is>
+      </c>
+      <c r="E947" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F947" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:47:56.849Z</t>
+        </is>
+      </c>
+      <c r="G947" t="n">
+        <v>154.9</v>
+      </c>
+      <c r="H947" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:47:45.076Z</t>
+        </is>
+      </c>
+      <c r="I947" t="n">
+        <v>190.9</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="n">
+        <v>65566</v>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>8072 Granville St</t>
+        </is>
+      </c>
+      <c r="D948" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.212495055855, 'Longitude': -123.14013004303}</t>
+        </is>
+      </c>
+      <c r="E948" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F948" t="inlineStr">
+        <is>
+          <t>2025-06-02T23:30:22.441Z</t>
+        </is>
+      </c>
+      <c r="G948" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H948" t="inlineStr">
+        <is>
+          <t>2025-06-02T14:34:40.218Z</t>
+        </is>
+      </c>
+      <c r="I948" t="n">
+        <v>171.9</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="n">
+        <v>65572</v>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>8686 Granville St</t>
+        </is>
+      </c>
+      <c r="D949" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.207280329467, 'Longitude': -123.140280246735}</t>
+        </is>
+      </c>
+      <c r="E949" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:05:00</t>
+        </is>
+      </c>
+      <c r="F949" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:25:12.898Z</t>
+        </is>
+      </c>
+      <c r="G949" t="n">
+        <v>158.9</v>
+      </c>
+      <c r="H949" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:33:09.257Z</t>
+        </is>
+      </c>
+      <c r="I949" t="n">
+        <v>208.9</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="n">
+        <v>65558</v>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>1390 E 33rd Ave</t>
+        </is>
+      </c>
+      <c r="D950" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.240045470021, 'Longitude': -123.076765537262}</t>
+        </is>
+      </c>
+      <c r="E950" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F950" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:04:51.746Z</t>
+        </is>
+      </c>
+      <c r="G950" t="n">
+        <v>143.9</v>
+      </c>
+      <c r="H950" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:17:10.564Z</t>
+        </is>
+      </c>
+      <c r="I950" t="n">
+        <v>168.9</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="n">
+        <v>83394</v>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>4064 Fraser St</t>
+        </is>
+      </c>
+      <c r="D951" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.248864, 'Longitude': -123.09002}</t>
+        </is>
+      </c>
+      <c r="E951" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F951" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:43:12.696Z</t>
+        </is>
+      </c>
+      <c r="G951" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H951" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:37:53.709Z</t>
+        </is>
+      </c>
+      <c r="I951" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="n">
+        <v>65573</v>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>1396 E 41st Ave</t>
+        </is>
+      </c>
+      <c r="D952" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.232593005895, 'Longitude': -123.07728856802}</t>
+        </is>
+      </c>
+      <c r="E952" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F952" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:44:57.862Z</t>
+        </is>
+      </c>
+      <c r="G952" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H952" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:42:32.503Z</t>
+        </is>
+      </c>
+      <c r="I952" t="n">
+        <v>190.9</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="n">
+        <v>80714</v>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Husky</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>4933 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D953" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2397388, 'Longitude': -123.065748}</t>
+        </is>
+      </c>
+      <c r="E953" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F953" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:38:58.731Z</t>
+        </is>
+      </c>
+      <c r="G953" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H953" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:56:29.929Z</t>
+        </is>
+      </c>
+      <c r="I953" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="n">
+        <v>65552</v>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>2001 Kingsway</t>
+        </is>
+      </c>
+      <c r="D954" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.245312771918, 'Longitude': -123.064910173416}</t>
+        </is>
+      </c>
+      <c r="E954" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F954" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:03:45.795Z</t>
+        </is>
+      </c>
+      <c r="G954" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H954" t="inlineStr">
+        <is>
+          <t>2025-06-02T06:13:11.802Z</t>
+        </is>
+      </c>
+      <c r="I954" t="n">
+        <v>184.9</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="n">
+        <v>65538</v>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>5252 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D955" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2372145, 'Longitude': -123.0650857}</t>
+        </is>
+      </c>
+      <c r="E955" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F955" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:26:38.751Z</t>
+        </is>
+      </c>
+      <c r="G955" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H955" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:58:07.469Z</t>
+        </is>
+      </c>
+      <c r="I955" t="n">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="n">
+        <v>90814</v>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>2277 Kingsway</t>
+        </is>
+      </c>
+      <c r="D956" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.242132845692, 'Longitude': -123.058204650879}</t>
+        </is>
+      </c>
+      <c r="E956" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F956" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:43:08.264Z</t>
+        </is>
+      </c>
+      <c r="G956" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H956" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:39:49.406Z</t>
+        </is>
+      </c>
+      <c r="I956" t="n">
+        <v>174.9</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="n">
+        <v>39768</v>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>5736 Main St</t>
+        </is>
+      </c>
+      <c r="D957" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2325708, 'Longitude': -123.1010069}</t>
+        </is>
+      </c>
+      <c r="E957" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F957" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:35:57.999Z</t>
+        </is>
+      </c>
+      <c r="G957" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H957" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:58:16.032Z</t>
+        </is>
+      </c>
+      <c r="I957" t="n">
+        <v>180.9</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="n">
+        <v>9710</v>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>1295 E 12th Ave</t>
+        </is>
+      </c>
+      <c r="D958" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.259878978744, 'Longitude': -123.078074455261}</t>
+        </is>
+      </c>
+      <c r="E958" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F958" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:41:08.748Z</t>
+        </is>
+      </c>
+      <c r="G958" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H958" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:41:08.780Z</t>
+        </is>
+      </c>
+      <c r="I958" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="n">
+        <v>99146</v>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Super Save Gas</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>1317 E 12th Ave</t>
+        </is>
+      </c>
+      <c r="D959" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.259758544957, 'Longitude': -123.077272474766}</t>
+        </is>
+      </c>
+      <c r="E959" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F959" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:40:52.924Z</t>
+        </is>
+      </c>
+      <c r="G959" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H959" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:40:52.955Z</t>
+        </is>
+      </c>
+      <c r="I959" t="n">
+        <v>176.9</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="n">
+        <v>65560</v>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>1289 E Broadway</t>
+        </is>
+      </c>
+      <c r="D960" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.262693682723, 'Longitude': -123.078117370605}</t>
+        </is>
+      </c>
+      <c r="E960" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F960" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:39:37.595Z</t>
+        </is>
+      </c>
+      <c r="G960" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H960" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:56:44.321Z</t>
+        </is>
+      </c>
+      <c r="I960" t="n">
+        <v>199.9</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="n">
+        <v>65557</v>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>2120 Grandview Hwy S</t>
+        </is>
+      </c>
+      <c r="D961" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2591601, 'Longitude': -123.0617495}</t>
+        </is>
+      </c>
+      <c r="E961" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F961" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:42:35.609Z</t>
+        </is>
+      </c>
+      <c r="G961" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="H961" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:42:35.640Z</t>
+        </is>
+      </c>
+      <c r="I961" t="n">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="n">
+        <v>71502</v>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>2748 Main St</t>
+        </is>
+      </c>
+      <c r="D962" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2604441, 'Longitude': -123.1005869}</t>
+        </is>
+      </c>
+      <c r="E962" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F962" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:32:52.042Z</t>
+        </is>
+      </c>
+      <c r="G962" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H962" t="inlineStr">
+        <is>
+          <t>2025-06-02T21:21:38.000Z</t>
+        </is>
+      </c>
+      <c r="I962" t="n">
+        <v>185.9</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="n">
+        <v>65559</v>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>6502 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D963" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.224996944057, 'Longitude': -123.065521717072}</t>
+        </is>
+      </c>
+      <c r="E963" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F963" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:18:01.663Z</t>
+        </is>
+      </c>
+      <c r="G963" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H963" t="inlineStr">
+        <is>
+          <t>2025-06-02T06:06:50.117Z</t>
+        </is>
+      </c>
+      <c r="I963" t="n">
+        <v>181.9</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="n">
+        <v>89943</v>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>6808 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D964" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2220242, 'Longitude': -123.0654247}</t>
+        </is>
+      </c>
+      <c r="E964" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F964" t="inlineStr">
+        <is>
+          <t>2025-06-02T23:52:00.867Z</t>
+        </is>
+      </c>
+      <c r="G964" t="n">
+        <v>157.9</v>
+      </c>
+      <c r="H964" t="inlineStr">
+        <is>
+          <t>2025-06-02T19:52:39.606Z</t>
+        </is>
+      </c>
+      <c r="I964" t="n">
+        <v>182.9</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="n">
+        <v>86880</v>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>7282 Knight St</t>
+        </is>
+      </c>
+      <c r="D965" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.218250007984, 'Longitude': -123.076816499233}</t>
+        </is>
+      </c>
+      <c r="E965" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F965" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:39:13.484Z</t>
+        </is>
+      </c>
+      <c r="G965" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H965" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:19:17.124Z</t>
+        </is>
+      </c>
+      <c r="I965" t="n">
+        <v>192.9</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="n">
+        <v>65537</v>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>2918 Kingsway</t>
+        </is>
+      </c>
+      <c r="D966" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.23608, 'Longitude': -123.0454858}</t>
+        </is>
+      </c>
+      <c r="E966" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F966" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:44:53.283Z</t>
+        </is>
+      </c>
+      <c r="G966" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H966" t="inlineStr">
+        <is>
+          <t>2025-06-02T18:09:25.796Z</t>
+        </is>
+      </c>
+      <c r="I966" t="n">
+        <v>185.9</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="n">
+        <v>65536</v>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>7309 Knight St</t>
+        </is>
+      </c>
+      <c r="D967" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2177761, 'Longitude': -123.0775405}</t>
+        </is>
+      </c>
+      <c r="E967" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F967" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:38:38.327Z</t>
+        </is>
+      </c>
+      <c r="G967" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H967" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:06:25.786Z</t>
+        </is>
+      </c>
+      <c r="I967" t="n">
+        <v>200.9</v>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="n">
+        <v>65535</v>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>2605 E 49th Ave</t>
+        </is>
+      </c>
+      <c r="D968" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2251291, 'Longitude': -123.0545048}</t>
+        </is>
+      </c>
+      <c r="E968" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F968" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:23:41.825Z</t>
+        </is>
+      </c>
+      <c r="G968" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H968" t="inlineStr">
+        <is>
+          <t>2025-06-01T15:18:20.433Z</t>
+        </is>
+      </c>
+      <c r="I968" t="n">
+        <v>185.9</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="n">
+        <v>65539</v>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>2902 Grandview Hwy</t>
+        </is>
+      </c>
+      <c r="D969" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2579053, 'Longitude': -123.0438464}</t>
+        </is>
+      </c>
+      <c r="E969" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:07:57</t>
+        </is>
+      </c>
+      <c r="F969" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:43:55.178Z</t>
+        </is>
+      </c>
+      <c r="G969" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="H969" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:43:55.193Z</t>
+        </is>
+      </c>
+      <c r="I969" t="n">
+        <v>184.9</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="n">
+        <v>77015</v>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Super Save Gas</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>6000 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D970" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169873456637, 'Longitude': -123.091178619746}</t>
+        </is>
+      </c>
+      <c r="E970" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F970" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:23:47.246Z</t>
+        </is>
+      </c>
+      <c r="G970" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H970" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:03.431Z</t>
+        </is>
+      </c>
+      <c r="I970" t="n">
+        <v>172.9</v>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="n">
+        <v>65511</v>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12011 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D971" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1923857, 'Longitude': -123.0911072}</t>
+        </is>
+      </c>
+      <c r="E971" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F971" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:48:16.615Z</t>
+        </is>
+      </c>
+      <c r="G971" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H971" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:13:20.720Z</t>
+        </is>
+      </c>
+      <c r="I971" t="n">
+        <v>183.9</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="n">
+        <v>86650</v>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>9100 Westminster Hwy</t>
+        </is>
+      </c>
+      <c r="D972" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169856952787, 'Longitude': -123.123961687088}</t>
+        </is>
+      </c>
+      <c r="E972" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F972" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:02:11.635Z</t>
+        </is>
+      </c>
+      <c r="G972" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H972" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:12.310Z</t>
+        </is>
+      </c>
+      <c r="I972" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="n">
+        <v>77218</v>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>5511 Garden City Rd</t>
+        </is>
+      </c>
+      <c r="D973" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.173339635958, 'Longitude': -123.124954104424}</t>
+        </is>
+      </c>
+      <c r="E973" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F973" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:02:26.913Z</t>
+        </is>
+      </c>
+      <c r="G973" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="H973" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:48.763Z</t>
+        </is>
+      </c>
+      <c r="I973" t="n">
+        <v>173.9</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="n">
+        <v>77228</v>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>9100 Cambie Rd</t>
+        </is>
+      </c>
+      <c r="D974" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1843249, 'Longitude': -123.1236078}</t>
+        </is>
+      </c>
+      <c r="E974" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F974" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:05:43.898Z</t>
+        </is>
+      </c>
+      <c r="G974" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H974" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:56.401Z</t>
+        </is>
+      </c>
+      <c r="I974" t="n">
+        <v>177.9</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="n">
+        <v>83384</v>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>9060 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D975" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.192001, 'Longitude': -123.124004}</t>
+        </is>
+      </c>
+      <c r="E975" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F975" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:05:44.748Z</t>
+        </is>
+      </c>
+      <c r="G975" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H975" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:19:06.116Z</t>
+        </is>
+      </c>
+      <c r="I975" t="n">
+        <v>189.9</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="n">
+        <v>77202</v>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>8151 Granville Ave</t>
+        </is>
+      </c>
+      <c r="D976" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.162989071149, 'Longitude': -123.134229183197}</t>
+        </is>
+      </c>
+      <c r="E976" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F976" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:02:12.113Z</t>
+        </is>
+      </c>
+      <c r="G976" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H976" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:50.548Z</t>
+        </is>
+      </c>
+      <c r="I976" t="n">
+        <v>174.9</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="n">
+        <v>77243</v>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>4651 No  3 Rd</t>
+        </is>
+      </c>
+      <c r="D977" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.179182137142, 'Longitude': -123.137152791023}</t>
+        </is>
+      </c>
+      <c r="E977" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F977" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:26:15.974Z</t>
+        </is>
+      </c>
+      <c r="G977" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H977" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:49.580Z</t>
+        </is>
+      </c>
+      <c r="I977" t="n">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="n">
+        <v>83387</v>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>710 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D978" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.21081995506, 'Longitude': -123.090755939484}</t>
+        </is>
+      </c>
+      <c r="E978" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F978" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:05:49.698Z</t>
+        </is>
+      </c>
+      <c r="G978" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H978" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:38:52.730Z</t>
+        </is>
+      </c>
+      <c r="I978" t="n">
+        <v>168.9</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="n">
+        <v>65551</v>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>688 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D979" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.210798928329, 'Longitude': -123.09152841568}</t>
+        </is>
+      </c>
+      <c r="E979" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F979" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:04:56.516Z</t>
+        </is>
+      </c>
+      <c r="G979" t="n">
+        <v>143.9</v>
+      </c>
+      <c r="H979" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:26:30.673Z</t>
+        </is>
+      </c>
+      <c r="I979" t="n">
+        <v>189.9</v>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="n">
+        <v>77235</v>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Domo</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4071 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D980" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.18409178594, 'Longitude': -123.136823830688}</t>
+        </is>
+      </c>
+      <c r="E980" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F980" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:56:50.025Z</t>
+        </is>
+      </c>
+      <c r="G980" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H980" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:55.514Z</t>
+        </is>
+      </c>
+      <c r="I980" t="n">
+        <v>174.9</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="n">
+        <v>82925</v>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>350 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D981" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.210245, 'Longitude': -123.099328}</t>
+        </is>
+      </c>
+      <c r="E981" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F981" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:36:35.417Z</t>
+        </is>
+      </c>
+      <c r="G981" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="H981" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:26:18.076Z</t>
+        </is>
+      </c>
+      <c r="I981" t="n">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="n">
+        <v>109205</v>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>11991 Steveston Hwy</t>
+        </is>
+      </c>
+      <c r="D982" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.133556536531, 'Longitude': -123.092424273491}</t>
+        </is>
+      </c>
+      <c r="E982" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F982" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:54:34.062Z</t>
+        </is>
+      </c>
+      <c r="G982" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H982" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:59:49.446Z</t>
+        </is>
+      </c>
+      <c r="I982" t="n">
+        <v>177.9</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="n">
+        <v>65540</v>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>196 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D983" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2106867, 'Longitude': -123.1027436}</t>
+        </is>
+      </c>
+      <c r="E983" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F983" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:24:57.964Z</t>
+        </is>
+      </c>
+      <c r="G983" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H983" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:10:24.281Z</t>
+        </is>
+      </c>
+      <c r="I983" t="n">
+        <v>180.9</v>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="n">
+        <v>65512</v>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>11131 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D984" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1328393, 'Longitude': -123.0926312}</t>
+        </is>
+      </c>
+      <c r="E984" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F984" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:38:58.300Z</t>
+        </is>
+      </c>
+      <c r="G984" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H984" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:47:48.317Z</t>
+        </is>
+      </c>
+      <c r="I984" t="n">
+        <v>204.9</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="n">
+        <v>77205</v>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7951 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D985" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1558882, 'Longitude': -123.1369625}</t>
+        </is>
+      </c>
+      <c r="E985" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F985" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:07:41.456Z</t>
+        </is>
+      </c>
+      <c r="G985" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H985" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:07:41.503Z</t>
+        </is>
+      </c>
+      <c r="I985" t="n">
+        <v>194.9</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="n">
+        <v>65536</v>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>7309 Knight St</t>
+        </is>
+      </c>
+      <c r="D986" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2177761, 'Longitude': -123.0775405}</t>
+        </is>
+      </c>
+      <c r="E986" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F986" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:38:38.327Z</t>
+        </is>
+      </c>
+      <c r="G986" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H986" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:06:25.786Z</t>
+        </is>
+      </c>
+      <c r="I986" t="n">
+        <v>200.9</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="n">
+        <v>86880</v>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>7282 Knight St</t>
+        </is>
+      </c>
+      <c r="D987" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.218250007984, 'Longitude': -123.076816499233}</t>
+        </is>
+      </c>
+      <c r="E987" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F987" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:39:13.484Z</t>
+        </is>
+      </c>
+      <c r="G987" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H987" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:19:17.124Z</t>
+        </is>
+      </c>
+      <c r="I987" t="n">
+        <v>192.9</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="n">
+        <v>65556</v>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>709 SW Marine Dr</t>
+        </is>
+      </c>
+      <c r="D988" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.20806537721, 'Longitude': -123.123285770416}</t>
+        </is>
+      </c>
+      <c r="E988" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F988" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:57:24.670Z</t>
+        </is>
+      </c>
+      <c r="G988" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H988" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:29:55.022Z</t>
+        </is>
+      </c>
+      <c r="I988" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="n">
+        <v>86937</v>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>8655 Boundary Rd</t>
+        </is>
+      </c>
+      <c r="D989" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.20476, 'Longitude': -123.02398}</t>
+        </is>
+      </c>
+      <c r="E989" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:10:53</t>
+        </is>
+      </c>
+      <c r="F989" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:27:11.402Z</t>
+        </is>
+      </c>
+      <c r="G989" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H989" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:17:07.989Z</t>
+        </is>
+      </c>
+      <c r="I989" t="n">
+        <v>202.9</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>65515</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>4011 Francis Rd</t>
+        </is>
+      </c>
+      <c r="D990" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.14867500071, 'Longitude': -123.180856704712}</t>
+        </is>
+      </c>
+      <c r="E990" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F990" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:53:55.755Z</t>
+        </is>
+      </c>
+      <c r="G990" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H990" t="inlineStr">
+        <is>
+          <t>2025-06-02T13:05:37.222Z</t>
+        </is>
+      </c>
+      <c r="I990" t="n">
+        <v>202.9</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>77205</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7951 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D991" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1558882, 'Longitude': -123.1369625}</t>
+        </is>
+      </c>
+      <c r="E991" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F991" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:07:41.456Z</t>
+        </is>
+      </c>
+      <c r="G991" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H991" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:07:41.503Z</t>
+        </is>
+      </c>
+      <c r="I991" t="n">
+        <v>194.9</v>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>77223</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>7991 No 1 Rd</t>
+        </is>
+      </c>
+      <c r="D992" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.155888686563, 'Longitude': -123.181414604187}</t>
+        </is>
+      </c>
+      <c r="E992" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F992" t="inlineStr">
+        <is>
+          <t>2025-06-02T23:35:20.958Z</t>
+        </is>
+      </c>
+      <c r="G992" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="H992" t="inlineStr">
+        <is>
+          <t>2025-06-02T16:33:00.598Z</t>
+        </is>
+      </c>
+      <c r="I992" t="n">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>65514</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>7980 Williams Rd</t>
+        </is>
+      </c>
+      <c r="D993" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.140582914547, 'Longitude': -123.137168884277}</t>
+        </is>
+      </c>
+      <c r="E993" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F993" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:41:06.147Z</t>
+        </is>
+      </c>
+      <c r="G993" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H993" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:07.419Z</t>
+        </is>
+      </c>
+      <c r="I993" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>77232</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5900 Westminster Hwy </t>
+        </is>
+      </c>
+      <c r="D994" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1698419, 'Longitude': -123.159282}</t>
+        </is>
+      </c>
+      <c r="E994" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F994" t="inlineStr">
+        <is>
+          <t>2025-06-03T03:16:37.540Z</t>
+        </is>
+      </c>
+      <c r="G994" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H994" t="inlineStr">
+        <is>
+          <t>2025-06-02T06:06:30.464Z</t>
+        </is>
+      </c>
+      <c r="I994" t="n">
+        <v>167.9</v>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>77202</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>8151 Granville Ave</t>
+        </is>
+      </c>
+      <c r="D995" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.162989071149, 'Longitude': -123.134229183197}</t>
+        </is>
+      </c>
+      <c r="E995" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F995" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:02:12.113Z</t>
+        </is>
+      </c>
+      <c r="G995" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H995" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:50.548Z</t>
+        </is>
+      </c>
+      <c r="I995" t="n">
+        <v>174.9</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>86650</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>9100 Westminster Hwy</t>
+        </is>
+      </c>
+      <c r="D996" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169856952787, 'Longitude': -123.123961687088}</t>
+        </is>
+      </c>
+      <c r="E996" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F996" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:02:11.635Z</t>
+        </is>
+      </c>
+      <c r="G996" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H996" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:12.310Z</t>
+        </is>
+      </c>
+      <c r="I996" t="n">
+        <v>179.9</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>77218</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>5511 Garden City Rd</t>
+        </is>
+      </c>
+      <c r="D997" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.173339635958, 'Longitude': -123.124954104424}</t>
+        </is>
+      </c>
+      <c r="E997" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F997" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:02:26.913Z</t>
+        </is>
+      </c>
+      <c r="G997" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="H997" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:48.763Z</t>
+        </is>
+      </c>
+      <c r="I997" t="n">
+        <v>173.9</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>4651 No  3 Rd</t>
+        </is>
+      </c>
+      <c r="D998" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.179182137142, 'Longitude': -123.137152791023}</t>
+        </is>
+      </c>
+      <c r="E998" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F998" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:26:15.974Z</t>
+        </is>
+      </c>
+      <c r="G998" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H998" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:49.580Z</t>
+        </is>
+      </c>
+      <c r="I998" t="n">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>77235</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Domo</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4071 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D999" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.18409178594, 'Longitude': -123.136823830688}</t>
+        </is>
+      </c>
+      <c r="E999" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F999" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:56:50.025Z</t>
+        </is>
+      </c>
+      <c r="G999" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H999" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:55.514Z</t>
+        </is>
+      </c>
+      <c r="I999" t="n">
+        <v>174.9</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>77228</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>9100 Cambie Rd</t>
+        </is>
+      </c>
+      <c r="D1000" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1843249, 'Longitude': -123.1236078}</t>
+        </is>
+      </c>
+      <c r="E1000" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1000" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:05:43.898Z</t>
+        </is>
+      </c>
+      <c r="G1000" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H1000" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:00:56.401Z</t>
+        </is>
+      </c>
+      <c r="I1000" t="n">
+        <v>177.9</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>69163</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>5111 Grant McConachie Way</t>
+        </is>
+      </c>
+      <c r="D1001" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.192919, 'Longitude': -123.166797}</t>
+        </is>
+      </c>
+      <c r="E1001" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1001" t="inlineStr">
+        <is>
+          <t>2025-06-02T23:24:55.689Z</t>
+        </is>
+      </c>
+      <c r="G1001" t="n">
+        <v>158.9</v>
+      </c>
+      <c r="H1001" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:58:37.237Z</t>
+        </is>
+      </c>
+      <c r="I1001" t="n">
+        <v>186.9</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>109205</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>11991 Steveston Hwy</t>
+        </is>
+      </c>
+      <c r="D1002" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.133556536531, 'Longitude': -123.092424273491}</t>
+        </is>
+      </c>
+      <c r="E1002" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1002" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:54:34.062Z</t>
+        </is>
+      </c>
+      <c r="G1002" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H1002" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:11:49.619Z</t>
+        </is>
+      </c>
+      <c r="I1002" t="n">
+        <v>177.9</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>65512</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>11131 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D1003" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1328393, 'Longitude': -123.0926312}</t>
+        </is>
+      </c>
+      <c r="E1003" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1003" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:38:58.300Z</t>
+        </is>
+      </c>
+      <c r="G1003" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H1003" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:11:55.768Z</t>
+        </is>
+      </c>
+      <c r="I1003" t="n">
+        <v>204.9</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>83384</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>9060 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D1004" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.192001, 'Longitude': -123.124004}</t>
+        </is>
+      </c>
+      <c r="E1004" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1004" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:05:44.748Z</t>
+        </is>
+      </c>
+      <c r="G1004" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H1004" t="inlineStr">
+        <is>
+          <t>2025-06-02T07:19:06.116Z</t>
+        </is>
+      </c>
+      <c r="I1004" t="n">
+        <v>189.9</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>77015</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Super Save Gas</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>6000 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169873456637, 'Longitude': -123.091178619746}</t>
+        </is>
+      </c>
+      <c r="E1005" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1005" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:13:38.211Z</t>
+        </is>
+      </c>
+      <c r="G1005" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H1005" t="inlineStr">
+        <is>
+          <t>2025-06-03T04:13:38.258Z</t>
+        </is>
+      </c>
+      <c r="I1005" t="n">
+        <v>170.9</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>107728</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>8884 Granville St</t>
+        </is>
+      </c>
+      <c r="D1006" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2054215, 'Longitude': -123.1401677}</t>
+        </is>
+      </c>
+      <c r="E1006" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1006" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:25:34.863Z</t>
+        </is>
+      </c>
+      <c r="G1006" t="n">
+        <v>154.9</v>
+      </c>
+      <c r="H1006" t="inlineStr">
+        <is>
+          <t>2025-06-02T04:39:28.772Z</t>
+        </is>
+      </c>
+      <c r="I1006" t="n">
+        <v>169.9</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>65572</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>8686 Granville St</t>
+        </is>
+      </c>
+      <c r="D1007" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.207280329467, 'Longitude': -123.140280246735}</t>
+        </is>
+      </c>
+      <c r="E1007" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1007" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:25:12.898Z</t>
+        </is>
+      </c>
+      <c r="G1007" t="n">
+        <v>158.9</v>
+      </c>
+      <c r="H1007" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:33:09.257Z</t>
+        </is>
+      </c>
+      <c r="I1007" t="n">
+        <v>208.9</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>65511</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12011 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D1008" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1923857, 'Longitude': -123.0911072}</t>
+        </is>
+      </c>
+      <c r="E1008" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1008" t="inlineStr">
+        <is>
+          <t>2025-06-03T02:48:16.615Z</t>
+        </is>
+      </c>
+      <c r="G1008" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H1008" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:13:20.720Z</t>
+        </is>
+      </c>
+      <c r="I1008" t="n">
+        <v>183.9</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>65556</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>709 SW Marine Dr</t>
+        </is>
+      </c>
+      <c r="D1009" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.20806537721, 'Longitude': -123.123285770416}</t>
+        </is>
+      </c>
+      <c r="E1009" t="inlineStr">
+        <is>
+          <t>2025-06-03 12:14:00</t>
+        </is>
+      </c>
+      <c r="F1009" t="inlineStr">
+        <is>
+          <t>2025-06-03T01:57:24.670Z</t>
+        </is>
+      </c>
+      <c r="G1009" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H1009" t="inlineStr">
+        <is>
+          <t>2025-06-02T22:29:55.022Z</t>
+        </is>
+      </c>
+      <c r="I1009" t="n">
         <v>179.9</v>
       </c>
     </row>

</xml_diff>